<commit_message>
added checkbox for insurance. Added new tables, added insurance coeffs to those.
</commit_message>
<xml_diff>
--- a/files/ku_tables.xlsx
+++ b/files/ku_tables.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Климат-здоровье" sheetId="1" r:id="rId1"/>
     <sheet name="Климат-возраст" sheetId="2" r:id="rId2"/>
     <sheet name="Назначение-здоровье" sheetId="3" r:id="rId3"/>
     <sheet name="Назначение-возраст" sheetId="4" r:id="rId4"/>
-    <sheet name="Питание-здоровье" sheetId="5" r:id="rId5"/>
-    <sheet name="Питание-возраст" sheetId="6" r:id="rId6"/>
+    <sheet name="Назначение-страховка" sheetId="7" r:id="rId5"/>
+    <sheet name="Питание-здоровье" sheetId="5" r:id="rId6"/>
+    <sheet name="Питание-возраст" sheetId="6" r:id="rId7"/>
+    <sheet name="Страховка-здоровье" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
   <si>
     <t>транзитные</t>
   </si>
@@ -101,6 +103,12 @@
   <si>
     <t>хорошее</t>
   </si>
+  <si>
+    <t>Есть</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
 </sst>
 </file>
 
@@ -146,6 +154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -194,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,7 +240,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,7 +1104,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,10 +1927,127 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.8</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,7 +2220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
@@ -2652,4 +2780,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>